<commit_message>
update, Default Target Preset
</commit_message>
<xml_diff>
--- a/project_manager/targets/default_targets/target_infos.xlsx
+++ b/project_manager/targets/default_targets/target_infos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="69">
   <si>
     <t xml:space="preserve">target_name</t>
   </si>
@@ -116,6 +116,7 @@
         <color rgb="FF000000"/>
         <rFont val="맑은 고딕"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">png</t>
     </r>
@@ -143,6 +144,7 @@
         <color rgb="FF000000"/>
         <rFont val="맑은 고딕"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">png</t>
     </r>
@@ -202,6 +204,12 @@
     <t xml:space="preserve">s22.jpg</t>
   </si>
   <si>
+    <t xml:space="preserve">s23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">default_target.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">Odroid-n2</t>
   </si>
   <si>
@@ -218,6 +226,45 @@
   </si>
   <si>
     <t xml:space="preserve">odroid-n2.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Odroid M1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Odroid_M1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rknn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rasberry Pi5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rasberry_Pi5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comma 3X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comma_3X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KT cloud</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KT_cloud</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amazon Web Services</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AWS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Google Cloud Platform</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GCP</t>
   </si>
 </sst>
 </file>
@@ -227,7 +274,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -249,6 +296,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -312,7 +366,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -322,6 +376,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -404,13 +462,13 @@
   </sheetPr>
   <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J17" activeCellId="0" sqref="J17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G26" activeCellId="0" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="3" style="0" width="15.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.78"/>
@@ -682,31 +740,209 @@
         <v>48</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="2" t="s">
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="H11" s="0" t="s">
+      <c r="D12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="G12" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
     <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
update, default target info
</commit_message>
<xml_diff>
--- a/project_manager/targets/default_targets/target_infos.xlsx
+++ b/project_manager/targets/default_targets/target_infos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="71">
   <si>
     <t xml:space="preserve">target_name</t>
   </si>
@@ -243,10 +243,16 @@
     <t xml:space="preserve">Rasberry_Pi5</t>
   </si>
   <si>
+    <t xml:space="preserve">tpu</t>
+  </si>
+  <si>
     <t xml:space="preserve">Comma 3X</t>
   </si>
   <si>
     <t xml:space="preserve">Comma_3X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adreno</t>
   </si>
   <si>
     <t xml:space="preserve">KT cloud</t>
@@ -274,7 +280,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -303,12 +309,6 @@
       <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="맑은 고딕"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -366,7 +366,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -379,7 +379,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -463,12 +467,12 @@
   <dimension ref="A1:H1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G26" activeCellId="0" sqref="G26"/>
+      <selection pane="topLeft" activeCell="F30" activeCellId="0" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="3" style="0" width="15.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.78"/>
@@ -788,13 +792,13 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="2" t="s">
         <v>58</v>
       </c>
       <c r="D13" s="2" t="s">
@@ -804,23 +808,23 @@
         <v>21</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="H13" s="0" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="4" t="s">
         <v>44</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -830,23 +834,23 @@
         <v>21</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="H14" s="0" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="B15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="B15" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D15" s="2" t="s">
@@ -856,7 +860,7 @@
         <v>21</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>54</v>
@@ -866,23 +870,23 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C16" s="3" t="s">
+      <c r="A16" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>53</v>
+        <v>4</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>54</v>
@@ -892,13 +896,13 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C17" s="3" t="s">
+      <c r="A17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D17" s="2" t="s">
@@ -918,13 +922,13 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C18" s="3" t="s">
+      <c r="A18" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D18" s="2" t="s">

</xml_diff>

<commit_message>
Change default target order and image
</commit_message>
<xml_diff>
--- a/project_manager/targets/default_targets/target_infos.xlsx
+++ b/project_manager/targets/default_targets/target_infos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="78">
   <si>
     <t xml:space="preserve">target_name</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t xml:space="preserve">image_file_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">order</t>
   </si>
   <si>
     <t xml:space="preserve">cloud</t>
@@ -207,7 +210,7 @@
     <t xml:space="preserve">s23</t>
   </si>
   <si>
-    <t xml:space="preserve">default_target.png</t>
+    <t xml:space="preserve">s23.jpg</t>
   </si>
   <si>
     <t xml:space="preserve">Odroid-n2</t>
@@ -237,6 +240,9 @@
     <t xml:space="preserve">rknn</t>
   </si>
   <si>
+    <t xml:space="preserve">OdroidM1.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">Rasberry Pi5</t>
   </si>
   <si>
@@ -246,6 +252,9 @@
     <t xml:space="preserve">tpu</t>
   </si>
   <si>
+    <t xml:space="preserve">RasberryPi5.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">Comma 3X</t>
   </si>
   <si>
@@ -255,22 +264,34 @@
     <t xml:space="preserve">adreno</t>
   </si>
   <si>
+    <t xml:space="preserve">comma-3x.jpg</t>
+  </si>
+  <si>
     <t xml:space="preserve">KT cloud</t>
   </si>
   <si>
     <t xml:space="preserve">KT_cloud</t>
   </si>
   <si>
+    <t xml:space="preserve">Kt_cloud.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">Amazon Web Services</t>
   </si>
   <si>
     <t xml:space="preserve">AWS</t>
   </si>
   <si>
+    <t xml:space="preserve">aws.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">Google Cloud Platform</t>
   </si>
   <si>
     <t xml:space="preserve">GCP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GCP.png</t>
   </si>
 </sst>
 </file>
@@ -464,10 +485,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H1048576"/>
+  <dimension ref="A1:I1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F30" activeCellId="0" sqref="F30"/>
+      <selection pane="topLeft" activeCell="I26" activeCellId="0" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -475,8 +496,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="3" style="0" width="15.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="21.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="8.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -504,447 +526,501 @@
       <c r="H1" s="0" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>9</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>49</v>
+        <v>60</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>49</v>
+        <v>64</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>49</v>
+        <v>68</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>49</v>
+        <v>71</v>
+      </c>
+      <c r="I16" s="0" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>49</v>
+        <v>74</v>
+      </c>
+      <c r="I17" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>49</v>
+        <v>77</v>
+      </c>
+      <c r="I18" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>